<commit_message>
validacion de anulacion y rehabilitacion de poliza
</commit_message>
<xml_diff>
--- a/Sura/DataSource - Cotización Hogar No Enlatada.xlsx
+++ b/Sura/DataSource - Cotización Hogar No Enlatada.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Irina Storozuk\Documents\Ranorex\RanorexStudio Projects\Sura\Sura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA9922FC-907F-4F21-80F9-1FC626A077C3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F944539-8762-4D55-B336-BD6F3F0750DA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -485,8 +485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -609,7 +609,7 @@
         <v>27</v>
       </c>
       <c r="O2">
-        <v>615</v>
+        <v>617</v>
       </c>
       <c r="P2" t="s">
         <v>25</v>

</xml_diff>